<commit_message>
Begin to implement xposed and sqlite
</commit_message>
<xml_diff>
--- a/design/database template.xlsx
+++ b/design/database template.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">status</t>
   </si>
   <si>
-    <t xml:space="preserve">businessName</t>
+    <t xml:space="preserve">user business</t>
   </si>
   <si>
     <t xml:space="preserve">clientName</t>
@@ -193,23 +193,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -286,189 +286,189 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>